<commit_message>
updates for manuscript revisions: NCBI taxonomy for LRM
</commit_message>
<xml_diff>
--- a/input_files/Differentially_abundant_families_all_methods.xlsx
+++ b/input_files/Differentially_abundant_families_all_methods.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgehrig/Desktop/Gehrig_et_al_sequencing_comparison/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jgehrig/Desktop/Gehrig_et_al_sequencing_comparison/input_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081975D2-44C5-1F45-ADB7-5698A6411318}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A460F287-07F6-CB44-BD5C-50E0EEE832CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35180" yWindow="500" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{E5D7D65F-DF48-AB4A-BC05-0C1F52C7D950}"/>
+    <workbookView xWindow="34440" yWindow="500" windowWidth="27640" windowHeight="16940" activeTab="1" xr2:uid="{E5D7D65F-DF48-AB4A-BC05-0C1F52C7D950}"/>
   </bookViews>
   <sheets>
     <sheet name="Significant" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1160" uniqueCount="143">
   <si>
     <t>feature</t>
   </si>
@@ -379,22 +379,91 @@
     <t>Paraprevotellaceae</t>
   </si>
   <si>
-    <t>Vallitaleaceae</t>
-  </si>
-  <si>
     <t>Podoviridae</t>
   </si>
   <si>
     <t>Saccharomycetaceae</t>
   </si>
   <si>
-    <t>CAG.1000</t>
-  </si>
-  <si>
-    <t>UBA1381</t>
-  </si>
-  <si>
-    <t>UBA1820</t>
+    <t>Thermoanaerobacterales.Family.III..Incertae.Sedis</t>
+  </si>
+  <si>
+    <t>Treponemataceae</t>
+  </si>
+  <si>
+    <t>Rhizobiaceae</t>
+  </si>
+  <si>
+    <t>Streptomycetaceae</t>
+  </si>
+  <si>
+    <t>Yersiniaceae</t>
+  </si>
+  <si>
+    <t>Roseobacteraceae</t>
+  </si>
+  <si>
+    <t>Bradyrhizobiaceae</t>
+  </si>
+  <si>
+    <t>Acetobacteraceae</t>
+  </si>
+  <si>
+    <t>Vibrionaceae</t>
+  </si>
+  <si>
+    <t>Pseudonocardiaceae</t>
+  </si>
+  <si>
+    <t>Eubacteriales.Family.XIII..Incertae.Sedis</t>
+  </si>
+  <si>
+    <t>Arcobacteraceae</t>
+  </si>
+  <si>
+    <t>Thermoanaerobacteraceae</t>
+  </si>
+  <si>
+    <t>Chitinophagaceae</t>
+  </si>
+  <si>
+    <t>Dysgonomonadaceae</t>
+  </si>
+  <si>
+    <t>Erwiniaceae</t>
+  </si>
+  <si>
+    <t>Pectobacteriaceae</t>
+  </si>
+  <si>
+    <t>Morganellaceae</t>
+  </si>
+  <si>
+    <t>Sphingomonadaceae</t>
+  </si>
+  <si>
+    <t>Sphingobacteriaceae</t>
+  </si>
+  <si>
+    <t>Flavobacteriaceae</t>
+  </si>
+  <si>
+    <t>Microbacteriaceae</t>
+  </si>
+  <si>
+    <t>Weeksellaceae</t>
+  </si>
+  <si>
+    <t>Moraxellaceae</t>
+  </si>
+  <si>
+    <t>Mycobacteriaceae</t>
+  </si>
+  <si>
+    <t>Coprobacillaceae</t>
+  </si>
+  <si>
+    <t>NCBI</t>
   </si>
 </sst>
 </file>
@@ -2422,9 +2491,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C6237D87-10B1-5845-80AC-3620C06FCCFB}">
-  <dimension ref="A1:J208"/>
+  <dimension ref="A1:J239"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O214" sqref="O214"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -6663,10 +6734,10 @@
         <v>10</v>
       </c>
       <c r="D133">
-        <v>0.19581586733707601</v>
+        <v>0.139564736381662</v>
       </c>
       <c r="E133">
-        <v>4.17404907680759E-2</v>
+        <v>3.0559636815192501E-2</v>
       </c>
       <c r="F133">
         <v>12</v>
@@ -6675,10 +6746,10 @@
         <v>12</v>
       </c>
       <c r="H133">
-        <v>5.3789788817383199E-3</v>
+        <v>6.01854451557175E-3</v>
       </c>
       <c r="I133">
-        <v>0.25281200744170101</v>
+        <v>0.475465016730168</v>
       </c>
       <c r="J133" t="s">
         <v>41</v>
@@ -6686,7 +6757,7 @@
     </row>
     <row r="134" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B134" t="s">
         <v>9</v>
@@ -6695,22 +6766,22 @@
         <v>10</v>
       </c>
       <c r="D134">
-        <v>0.86642572003449003</v>
+        <v>-0.26546785152162999</v>
       </c>
       <c r="E134">
-        <v>0.49031235373300502</v>
+        <v>0.106384861887728</v>
       </c>
       <c r="F134">
         <v>12</v>
       </c>
       <c r="G134">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H134">
-        <v>0.107659504516424</v>
+        <v>5.4800751705708903E-2</v>
       </c>
       <c r="I134">
-        <v>0.87048372331822099</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J134" t="s">
         <v>41</v>
@@ -6718,7 +6789,7 @@
     </row>
     <row r="135" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="B135" t="s">
         <v>9</v>
@@ -6727,22 +6798,22 @@
         <v>10</v>
       </c>
       <c r="D135">
-        <v>-0.223734954254422</v>
+        <v>7.3363181391088703E-2</v>
       </c>
       <c r="E135">
-        <v>0.124241549740361</v>
+        <v>3.02828761061774E-2</v>
       </c>
       <c r="F135">
         <v>12</v>
       </c>
       <c r="G135">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H135">
-        <v>0.13162090059006601</v>
+        <v>5.9925186931682403E-2</v>
       </c>
       <c r="I135">
-        <v>0.87048372331822099</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J135" t="s">
         <v>41</v>
@@ -6750,7 +6821,7 @@
     </row>
     <row r="136" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
-        <v>79</v>
+        <v>14</v>
       </c>
       <c r="B136" t="s">
         <v>9</v>
@@ -6759,22 +6830,22 @@
         <v>10</v>
       </c>
       <c r="D136">
-        <v>0.17387474985600901</v>
+        <v>-0.124383000090573</v>
       </c>
       <c r="E136">
-        <v>9.2044116217324598E-2</v>
+        <v>5.9479310504789502E-2</v>
       </c>
       <c r="F136">
         <v>12</v>
       </c>
       <c r="G136">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H136">
-        <v>0.117505189403265</v>
+        <v>9.0761714031872595E-2</v>
       </c>
       <c r="I136">
-        <v>0.87048372331822099</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J136" t="s">
         <v>41</v>
@@ -6782,7 +6853,7 @@
     </row>
     <row r="137" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
-        <v>31</v>
+        <v>116</v>
       </c>
       <c r="B137" t="s">
         <v>9</v>
@@ -6791,22 +6862,22 @@
         <v>10</v>
       </c>
       <c r="D137">
-        <v>7.30158380805115E-2</v>
+        <v>0.139343786470566</v>
       </c>
       <c r="E137">
-        <v>2.6623616935170898E-2</v>
+        <v>6.7298659654474693E-2</v>
       </c>
       <c r="F137">
         <v>12</v>
       </c>
       <c r="G137">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="H137">
-        <v>4.0669974695830099E-2</v>
+        <v>9.3176927313967303E-2</v>
       </c>
       <c r="I137">
-        <v>0.87048372331822099</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J137" t="s">
         <v>41</v>
@@ -6814,7 +6885,7 @@
     </row>
     <row r="138" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
-        <v>39</v>
+        <v>117</v>
       </c>
       <c r="B138" t="s">
         <v>9</v>
@@ -6823,22 +6894,22 @@
         <v>10</v>
       </c>
       <c r="D138">
-        <v>0.437132456522206</v>
+        <v>0.114301143968284</v>
       </c>
       <c r="E138">
-        <v>0.25579789078646697</v>
+        <v>6.0663034530339999E-2</v>
       </c>
       <c r="F138">
         <v>12</v>
       </c>
       <c r="G138">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="H138">
-        <v>0.14816744226693099</v>
+        <v>0.118237526178994</v>
       </c>
       <c r="I138">
-        <v>0.87048372331822099</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J138" t="s">
         <v>41</v>
@@ -6846,7 +6917,7 @@
     </row>
     <row r="139" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>14</v>
+        <v>118</v>
       </c>
       <c r="B139" t="s">
         <v>9</v>
@@ -6855,22 +6926,22 @@
         <v>10</v>
       </c>
       <c r="D139">
-        <v>-0.37267791990240101</v>
+        <v>4.2117687349772899E-2</v>
       </c>
       <c r="E139">
-        <v>0.176703136438702</v>
+        <v>2.4959222363892499E-2</v>
       </c>
       <c r="F139">
         <v>12</v>
       </c>
       <c r="G139">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H139">
-        <v>8.8727337838662004E-2</v>
+        <v>0.15231946286280801</v>
       </c>
       <c r="I139">
-        <v>0.87048372331822099</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J139" t="s">
         <v>41</v>
@@ -6878,7 +6949,7 @@
     </row>
     <row r="140" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="B140" t="s">
         <v>9</v>
@@ -6887,22 +6958,22 @@
         <v>10</v>
       </c>
       <c r="D140">
-        <v>0.25156367751659497</v>
+        <v>7.8731034857077206E-2</v>
       </c>
       <c r="E140">
-        <v>0.13081386819805299</v>
+        <v>4.7692982934434899E-2</v>
       </c>
       <c r="F140">
         <v>12</v>
       </c>
       <c r="G140">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H140">
-        <v>0.112485658204144</v>
+        <v>0.15969333463182001</v>
       </c>
       <c r="I140">
-        <v>0.87048372331822099</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J140" t="s">
         <v>41</v>
@@ -6910,7 +6981,7 @@
     </row>
     <row r="141" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
-        <v>15</v>
+        <v>81</v>
       </c>
       <c r="B141" t="s">
         <v>9</v>
@@ -6919,22 +6990,22 @@
         <v>10</v>
       </c>
       <c r="D141">
-        <v>-0.15161705869608399</v>
+        <v>0.102507655364081</v>
       </c>
       <c r="E141">
-        <v>0.12786128742835701</v>
+        <v>6.4851244595140106E-2</v>
       </c>
       <c r="F141">
         <v>12</v>
       </c>
       <c r="G141">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H141">
-        <v>0.28897915213179998</v>
+        <v>0.165048789663226</v>
       </c>
       <c r="I141">
-        <v>0.90546801001297395</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J141" t="s">
         <v>41</v>
@@ -6942,7 +7013,7 @@
     </row>
     <row r="142" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
-        <v>85</v>
+        <v>67</v>
       </c>
       <c r="B142" t="s">
         <v>9</v>
@@ -6951,22 +7022,22 @@
         <v>10</v>
       </c>
       <c r="D142">
-        <v>8.4721974286027305E-2</v>
+        <v>0.103587897375417</v>
       </c>
       <c r="E142">
-        <v>6.9125463294513606E-2</v>
+        <v>6.5560965172079502E-2</v>
       </c>
       <c r="F142">
         <v>12</v>
       </c>
       <c r="G142">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H142">
-        <v>0.27491535345925899</v>
+        <v>0.16518268798694999</v>
       </c>
       <c r="I142">
-        <v>0.90546801001297395</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J142" t="s">
         <v>41</v>
@@ -6974,7 +7045,7 @@
     </row>
     <row r="143" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="B143" t="s">
         <v>9</v>
@@ -6983,22 +7054,22 @@
         <v>10</v>
       </c>
       <c r="D143">
-        <v>0.44059452564892898</v>
+        <v>0.13354172421250801</v>
       </c>
       <c r="E143">
-        <v>0.30649605830211502</v>
+        <v>8.2765159381376005E-2</v>
       </c>
       <c r="F143">
         <v>12</v>
       </c>
       <c r="G143">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="H143">
-        <v>0.18111551083279001</v>
+        <v>0.16755504119718301</v>
       </c>
       <c r="I143">
-        <v>0.90546801001297395</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J143" t="s">
         <v>41</v>
@@ -7006,7 +7077,7 @@
     </row>
     <row r="144" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
-        <v>78</v>
+        <v>31</v>
       </c>
       <c r="B144" t="s">
         <v>9</v>
@@ -7015,10 +7086,10 @@
         <v>10</v>
       </c>
       <c r="D144">
-        <v>-0.15504612338478799</v>
+        <v>4.2547926185947701E-2</v>
       </c>
       <c r="E144">
-        <v>0.108591128750264</v>
+        <v>2.63753644530914E-2</v>
       </c>
       <c r="F144">
         <v>12</v>
@@ -7027,10 +7098,10 @@
         <v>12</v>
       </c>
       <c r="H144">
-        <v>0.212709671428951</v>
+        <v>0.16762683507290099</v>
       </c>
       <c r="I144">
-        <v>0.90546801001297395</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J144" t="s">
         <v>41</v>
@@ -7038,7 +7109,7 @@
     </row>
     <row r="145" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
-        <v>34</v>
+        <v>70</v>
       </c>
       <c r="B145" t="s">
         <v>9</v>
@@ -7047,10 +7118,10 @@
         <v>10</v>
       </c>
       <c r="D145">
-        <v>5.9991503418837397E-2</v>
+        <v>9.6105118384136504E-2</v>
       </c>
       <c r="E145">
-        <v>4.35346155981466E-2</v>
+        <v>5.9634924037598201E-2</v>
       </c>
       <c r="F145">
         <v>12</v>
@@ -7059,10 +7130,10 @@
         <v>12</v>
       </c>
       <c r="H145">
-        <v>0.22667531913844399</v>
+        <v>0.16797527641394</v>
       </c>
       <c r="I145">
-        <v>0.90546801001297395</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J145" t="s">
         <v>41</v>
@@ -7070,7 +7141,7 @@
     </row>
     <row r="146" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
-        <v>97</v>
+        <v>25</v>
       </c>
       <c r="B146" t="s">
         <v>9</v>
@@ -7079,22 +7150,22 @@
         <v>10</v>
       </c>
       <c r="D146">
-        <v>0.22865701482592801</v>
+        <v>-0.13170333985232099</v>
       </c>
       <c r="E146">
-        <v>0.168141674103262</v>
+        <v>8.3463863245199096E-2</v>
       </c>
       <c r="F146">
         <v>12</v>
       </c>
       <c r="G146">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H146">
-        <v>0.23196555976647701</v>
+        <v>0.175402387557448</v>
       </c>
       <c r="I146">
-        <v>0.90546801001297395</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J146" t="s">
         <v>41</v>
@@ -7102,7 +7173,7 @@
     </row>
     <row r="147" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>100</v>
+        <v>40</v>
       </c>
       <c r="B147" t="s">
         <v>9</v>
@@ -7111,10 +7182,10 @@
         <v>10</v>
       </c>
       <c r="D147">
-        <v>7.3904719801569693E-2</v>
+        <v>0.44054354141239299</v>
       </c>
       <c r="E147">
-        <v>5.9757395837815801E-2</v>
+        <v>0.30272821497867503</v>
       </c>
       <c r="F147">
         <v>12</v>
@@ -7123,10 +7194,10 @@
         <v>12</v>
       </c>
       <c r="H147">
-        <v>0.27110058125570902</v>
+        <v>0.176263636958854</v>
       </c>
       <c r="I147">
-        <v>0.90546801001297395</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J147" t="s">
         <v>41</v>
@@ -7134,7 +7205,7 @@
     </row>
     <row r="148" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="B148" t="s">
         <v>9</v>
@@ -7143,22 +7214,22 @@
         <v>10</v>
       </c>
       <c r="D148">
-        <v>-0.446257050990361</v>
+        <v>0.12344108225370801</v>
       </c>
       <c r="E148">
-        <v>0.43428659726319502</v>
+        <v>8.1711758046840402E-2</v>
       </c>
       <c r="F148">
         <v>12</v>
       </c>
       <c r="G148">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H148">
-        <v>0.328368675122861</v>
+        <v>0.19125926108793201</v>
       </c>
       <c r="I148">
-        <v>0.90784280769261505</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J148" t="s">
         <v>41</v>
@@ -7166,7 +7237,7 @@
     </row>
     <row r="149" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
-        <v>108</v>
+        <v>19</v>
       </c>
       <c r="B149" t="s">
         <v>9</v>
@@ -7175,22 +7246,22 @@
         <v>10</v>
       </c>
       <c r="D149">
-        <v>0.35836019299133398</v>
+        <v>0.66767732968811599</v>
       </c>
       <c r="E149">
-        <v>0.32200332067061999</v>
+        <v>0.47754632190901503</v>
       </c>
       <c r="F149">
         <v>12</v>
       </c>
       <c r="G149">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H149">
-        <v>0.31637053667745602</v>
+        <v>0.192306432612284</v>
       </c>
       <c r="I149">
-        <v>0.90784280769261505</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J149" t="s">
         <v>41</v>
@@ -7198,7 +7269,7 @@
     </row>
     <row r="150" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="B150" t="s">
         <v>9</v>
@@ -7207,10 +7278,10 @@
         <v>10</v>
       </c>
       <c r="D150">
-        <v>2.3453019286532598E-2</v>
+        <v>7.8900325683293901E-2</v>
       </c>
       <c r="E150">
-        <v>3.80089200402993E-2</v>
+        <v>5.3948670398524301E-2</v>
       </c>
       <c r="F150">
         <v>12</v>
@@ -7219,10 +7290,10 @@
         <v>12</v>
       </c>
       <c r="H150">
-        <v>0.56421926881380002</v>
+        <v>0.20346062696618999</v>
       </c>
       <c r="I150">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J150" t="s">
         <v>41</v>
@@ -7230,7 +7301,7 @@
     </row>
     <row r="151" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="B151" t="s">
         <v>9</v>
@@ -7239,22 +7310,22 @@
         <v>10</v>
       </c>
       <c r="D151">
-        <v>5.9428304420025703E-2</v>
+        <v>0.148204829466341</v>
       </c>
       <c r="E151">
-        <v>8.7634384100426094E-2</v>
+        <v>0.10290755295512299</v>
       </c>
       <c r="F151">
         <v>12</v>
       </c>
       <c r="G151">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="H151">
-        <v>0.52779135467569205</v>
+        <v>0.209366467009097</v>
       </c>
       <c r="I151">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J151" t="s">
         <v>41</v>
@@ -7262,7 +7333,7 @@
     </row>
     <row r="152" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
-        <v>17</v>
+        <v>78</v>
       </c>
       <c r="B152" t="s">
         <v>9</v>
@@ -7271,10 +7342,10 @@
         <v>10</v>
       </c>
       <c r="D152">
-        <v>-8.9061421206741001E-2</v>
+        <v>-0.15565329126102001</v>
       </c>
       <c r="E152">
-        <v>0.13576627378599601</v>
+        <v>0.10884827495150901</v>
       </c>
       <c r="F152">
         <v>12</v>
@@ -7283,10 +7354,10 @@
         <v>12</v>
       </c>
       <c r="H152">
-        <v>0.54081174856443304</v>
+        <v>0.212110365975968</v>
       </c>
       <c r="I152">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J152" t="s">
         <v>41</v>
@@ -7294,7 +7365,7 @@
     </row>
     <row r="153" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
-        <v>61</v>
+        <v>97</v>
       </c>
       <c r="B153" t="s">
         <v>9</v>
@@ -7303,10 +7374,10 @@
         <v>10</v>
       </c>
       <c r="D153">
-        <v>6.3368746033189496E-2</v>
+        <v>0.127861313018481</v>
       </c>
       <c r="E153">
-        <v>7.2741334230218002E-2</v>
+        <v>9.0575129307193095E-2</v>
       </c>
       <c r="F153">
         <v>12</v>
@@ -7315,10 +7386,10 @@
         <v>12</v>
       </c>
       <c r="H153">
-        <v>0.42351784855256802</v>
+        <v>0.217133875115116</v>
       </c>
       <c r="I153">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J153" t="s">
         <v>41</v>
@@ -7326,7 +7397,7 @@
     </row>
     <row r="154" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
-        <v>63</v>
+        <v>16</v>
       </c>
       <c r="B154" t="s">
         <v>9</v>
@@ -7335,22 +7406,22 @@
         <v>10</v>
       </c>
       <c r="D154">
-        <v>9.5691742076693898E-2</v>
+        <v>3.6969696659237897E-2</v>
       </c>
       <c r="E154">
-        <v>0.11249135466189999</v>
+        <v>2.65729833969858E-2</v>
       </c>
       <c r="F154">
         <v>12</v>
       </c>
       <c r="G154">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H154">
-        <v>0.43379529595522598</v>
+        <v>0.22287950042045801</v>
       </c>
       <c r="I154">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J154" t="s">
         <v>41</v>
@@ -7358,7 +7429,7 @@
     </row>
     <row r="155" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
-        <v>80</v>
+        <v>120</v>
       </c>
       <c r="B155" t="s">
         <v>9</v>
@@ -7367,22 +7438,22 @@
         <v>10</v>
       </c>
       <c r="D155">
-        <v>0.14630680958487199</v>
+        <v>6.8866527292745505E-2</v>
       </c>
       <c r="E155">
-        <v>0.176558657159925</v>
+        <v>4.96617348210305E-2</v>
       </c>
       <c r="F155">
         <v>12</v>
       </c>
       <c r="G155">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="H155">
-        <v>0.445039497139324</v>
+        <v>0.22417425785990699</v>
       </c>
       <c r="I155">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J155" t="s">
         <v>41</v>
@@ -7390,7 +7461,7 @@
     </row>
     <row r="156" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
-        <v>66</v>
+        <v>121</v>
       </c>
       <c r="B156" t="s">
         <v>9</v>
@@ -7399,22 +7470,22 @@
         <v>10</v>
       </c>
       <c r="D156">
-        <v>7.42511425967744E-2</v>
+        <v>7.2959917793406007E-2</v>
       </c>
       <c r="E156">
-        <v>9.64750950324538E-2</v>
+        <v>5.3632253011292499E-2</v>
       </c>
       <c r="F156">
         <v>12</v>
       </c>
       <c r="G156">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H156">
-        <v>0.4762807098504</v>
+        <v>0.23182765500165001</v>
       </c>
       <c r="I156">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J156" t="s">
         <v>41</v>
@@ -7422,7 +7493,7 @@
     </row>
     <row r="157" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
-        <v>111</v>
+        <v>122</v>
       </c>
       <c r="B157" t="s">
         <v>9</v>
@@ -7431,22 +7502,22 @@
         <v>10</v>
       </c>
       <c r="D157">
-        <v>0.176383172749948</v>
+        <v>6.6068750104611204E-2</v>
       </c>
       <c r="E157">
-        <v>0.22788921876541701</v>
+        <v>5.4126868494604602E-2</v>
       </c>
       <c r="F157">
         <v>12</v>
       </c>
       <c r="G157">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H157">
-        <v>0.47392676452757398</v>
+        <v>0.27664584061629799</v>
       </c>
       <c r="I157">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J157" t="s">
         <v>41</v>
@@ -7454,7 +7525,7 @@
     </row>
     <row r="158" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
-        <v>92</v>
+        <v>123</v>
       </c>
       <c r="B158" t="s">
         <v>9</v>
@@ -7463,22 +7534,22 @@
         <v>10</v>
       </c>
       <c r="D158">
-        <v>0.34729322439605498</v>
+        <v>6.8260297573573298E-2</v>
       </c>
       <c r="E158">
-        <v>0.39507125463311599</v>
+        <v>5.59833391070481E-2</v>
       </c>
       <c r="F158">
         <v>12</v>
       </c>
       <c r="G158">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H158">
-        <v>0.41960015524539501</v>
+        <v>0.27710827052210102</v>
       </c>
       <c r="I158">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J158" t="s">
         <v>41</v>
@@ -7486,7 +7557,7 @@
     </row>
     <row r="159" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
-        <v>33</v>
+        <v>124</v>
       </c>
       <c r="B159" t="s">
         <v>9</v>
@@ -7495,22 +7566,22 @@
         <v>10</v>
       </c>
       <c r="D159">
-        <v>5.0466642090951898E-2</v>
+        <v>0.13065631384080201</v>
       </c>
       <c r="E159">
-        <v>6.0390455916155397E-2</v>
+        <v>0.117130887944302</v>
       </c>
       <c r="F159">
         <v>12</v>
       </c>
       <c r="G159">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="H159">
-        <v>0.44143090574516097</v>
+        <v>0.29073589773386299</v>
       </c>
       <c r="I159">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J159" t="s">
         <v>41</v>
@@ -7518,7 +7589,7 @@
     </row>
     <row r="160" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
-        <v>114</v>
+        <v>125</v>
       </c>
       <c r="B160" t="s">
         <v>9</v>
@@ -7527,22 +7598,22 @@
         <v>10</v>
       </c>
       <c r="D160">
-        <v>6.0828507185377398E-2</v>
+        <v>7.4228179032825095E-2</v>
       </c>
       <c r="E160">
-        <v>8.9042468921747595E-2</v>
+        <v>6.78361763368419E-2</v>
       </c>
       <c r="F160">
         <v>12</v>
       </c>
       <c r="G160">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="H160">
-        <v>0.52488066549653001</v>
+        <v>0.323745534628053</v>
       </c>
       <c r="I160">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J160" t="s">
         <v>41</v>
@@ -7550,7 +7621,7 @@
     </row>
     <row r="161" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
-        <v>96</v>
+        <v>126</v>
       </c>
       <c r="B161" t="s">
         <v>9</v>
@@ -7559,22 +7630,22 @@
         <v>10</v>
       </c>
       <c r="D161">
-        <v>-0.120648465502794</v>
+        <v>0.11986373460888999</v>
       </c>
       <c r="E161">
-        <v>0.187679825171782</v>
+        <v>0.109542689796508</v>
       </c>
       <c r="F161">
         <v>12</v>
       </c>
       <c r="G161">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H161">
-        <v>0.54864140478316004</v>
+        <v>0.32374859051643301</v>
       </c>
       <c r="I161">
-        <v>0.91442433221546904</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J161" t="s">
         <v>41</v>
@@ -7582,7 +7653,7 @@
     </row>
     <row r="162" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
-        <v>44</v>
+        <v>127</v>
       </c>
       <c r="B162" t="s">
         <v>9</v>
@@ -7591,22 +7662,22 @@
         <v>10</v>
       </c>
       <c r="D162">
-        <v>2.2803988408570099E-2</v>
+        <v>5.01716659439993E-2</v>
       </c>
       <c r="E162">
-        <v>0.13050325212840899</v>
+        <v>5.0171665943996899E-2</v>
       </c>
       <c r="F162">
         <v>12</v>
       </c>
       <c r="G162">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H162">
-        <v>0.86814017596087401</v>
+        <v>0.34089313230211299</v>
       </c>
       <c r="I162">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J162" t="s">
         <v>41</v>
@@ -7614,7 +7685,7 @@
     </row>
     <row r="163" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="B163" t="s">
         <v>9</v>
@@ -7623,22 +7694,22 @@
         <v>10</v>
       </c>
       <c r="D163">
-        <v>-4.3152069411006501E-2</v>
+        <v>5.0171665943998099E-2</v>
       </c>
       <c r="E163">
-        <v>0.111754695003542</v>
+        <v>5.0171665943996899E-2</v>
       </c>
       <c r="F163">
         <v>12</v>
       </c>
       <c r="G163">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H163">
-        <v>0.71528311066156203</v>
+        <v>0.34089313230212398</v>
       </c>
       <c r="I163">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J163" t="s">
         <v>41</v>
@@ -7646,7 +7717,7 @@
     </row>
     <row r="164" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
-        <v>99</v>
+        <v>39</v>
       </c>
       <c r="B164" t="s">
         <v>9</v>
@@ -7655,22 +7726,22 @@
         <v>10</v>
       </c>
       <c r="D164">
-        <v>1.86120702121386E-2</v>
+        <v>5.0171665943998099E-2</v>
       </c>
       <c r="E164">
-        <v>4.2343349508404002E-2</v>
+        <v>5.0171665943996899E-2</v>
       </c>
       <c r="F164">
         <v>12</v>
       </c>
       <c r="G164">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H164">
-        <v>0.67861025807084996</v>
+        <v>0.34089313230212398</v>
       </c>
       <c r="I164">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J164" t="s">
         <v>41</v>
@@ -7678,7 +7749,7 @@
     </row>
     <row r="165" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="B165" t="s">
         <v>9</v>
@@ -7687,22 +7758,22 @@
         <v>10</v>
       </c>
       <c r="D165">
-        <v>-5.85095374801477E-2</v>
+        <v>-5.0171665943996899E-2</v>
       </c>
       <c r="E165">
-        <v>0.24687237668721301</v>
+        <v>5.0171665943996899E-2</v>
       </c>
       <c r="F165">
         <v>12</v>
       </c>
       <c r="G165">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H165">
-        <v>0.822058545518354</v>
+        <v>0.34089313230213503</v>
       </c>
       <c r="I165">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J165" t="s">
         <v>41</v>
@@ -7710,7 +7781,7 @@
     </row>
     <row r="166" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="B166" t="s">
         <v>9</v>
@@ -7719,22 +7790,22 @@
         <v>10</v>
       </c>
       <c r="D166">
-        <v>3.3724357497170801E-2</v>
+        <v>-5.0171665943995698E-2</v>
       </c>
       <c r="E166">
-        <v>0.157861569005257</v>
+        <v>5.0171665943996899E-2</v>
       </c>
       <c r="F166">
         <v>12</v>
       </c>
       <c r="G166">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H166">
-        <v>0.83927178257877799</v>
+        <v>0.340893132302164</v>
       </c>
       <c r="I166">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J166" t="s">
         <v>41</v>
@@ -7742,7 +7813,7 @@
     </row>
     <row r="167" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
-        <v>101</v>
+        <v>131</v>
       </c>
       <c r="B167" t="s">
         <v>9</v>
@@ -7751,22 +7822,22 @@
         <v>10</v>
       </c>
       <c r="D167">
-        <v>-1.1154191003529299E-2</v>
+        <v>5.01716659439993E-2</v>
       </c>
       <c r="E167">
-        <v>6.9568568180445406E-2</v>
+        <v>5.0171665943996802E-2</v>
       </c>
       <c r="F167">
         <v>12</v>
       </c>
       <c r="G167">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H167">
-        <v>0.87889446471300903</v>
+        <v>0.340893132302171</v>
       </c>
       <c r="I167">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J167" t="s">
         <v>41</v>
@@ -7774,7 +7845,7 @@
     </row>
     <row r="168" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="B168" t="s">
         <v>9</v>
@@ -7783,22 +7854,22 @@
         <v>10</v>
       </c>
       <c r="D168">
-        <v>-1.4025139204952901E-2</v>
+        <v>5.0171665943994498E-2</v>
       </c>
       <c r="E168">
-        <v>4.9588355921331199E-2</v>
+        <v>5.0171665942946399E-2</v>
       </c>
       <c r="F168">
         <v>12</v>
       </c>
       <c r="G168">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H168">
-        <v>0.78864136265004903</v>
+        <v>0.34089325282877603</v>
       </c>
       <c r="I168">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J168" t="s">
         <v>41</v>
@@ -7806,7 +7877,7 @@
     </row>
     <row r="169" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
-        <v>30</v>
+        <v>55</v>
       </c>
       <c r="B169" t="s">
         <v>9</v>
@@ -7815,22 +7886,22 @@
         <v>10</v>
       </c>
       <c r="D169">
-        <v>-0.17516308731717001</v>
+        <v>-5.0171665943998099E-2</v>
       </c>
       <c r="E169">
-        <v>0.341947999432404</v>
+        <v>5.0171665661586901E-2</v>
       </c>
       <c r="F169">
         <v>12</v>
       </c>
       <c r="G169">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H169">
-        <v>0.63029275892848802</v>
+        <v>0.34089369509255701</v>
       </c>
       <c r="I169">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J169" t="s">
         <v>41</v>
@@ -7838,7 +7909,7 @@
     </row>
     <row r="170" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
-        <v>25</v>
+        <v>132</v>
       </c>
       <c r="B170" t="s">
         <v>9</v>
@@ -7847,22 +7918,22 @@
         <v>10</v>
       </c>
       <c r="D170">
-        <v>0.13080707981267101</v>
+        <v>5.0171665943994498E-2</v>
       </c>
       <c r="E170">
-        <v>0.32195569008706698</v>
+        <v>5.0171665660654001E-2</v>
       </c>
       <c r="F170">
         <v>12</v>
       </c>
       <c r="G170">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H170">
-        <v>0.70133527547492802</v>
+        <v>0.34089490269185302</v>
       </c>
       <c r="I170">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J170" t="s">
         <v>41</v>
@@ -7870,7 +7941,7 @@
     </row>
     <row r="171" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
-        <v>104</v>
+        <v>115</v>
       </c>
       <c r="B171" t="s">
         <v>9</v>
@@ -7879,22 +7950,22 @@
         <v>10</v>
       </c>
       <c r="D171">
-        <v>2.0649734944402202E-2</v>
+        <v>5.0171665943998099E-2</v>
       </c>
       <c r="E171">
-        <v>7.2281593168987301E-2</v>
+        <v>5.01716655337291E-2</v>
       </c>
       <c r="F171">
         <v>12</v>
       </c>
       <c r="G171">
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="H171">
-        <v>0.78657684992289401</v>
+        <v>0.34089495717218499</v>
       </c>
       <c r="I171">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J171" t="s">
         <v>41</v>
@@ -7902,7 +7973,7 @@
     </row>
     <row r="172" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="B172" t="s">
         <v>9</v>
@@ -7911,22 +7982,22 @@
         <v>10</v>
       </c>
       <c r="D172">
-        <v>7.4718203683888901E-2</v>
+        <v>5.0171665943995698E-2</v>
       </c>
       <c r="E172">
-        <v>0.14369886703438001</v>
+        <v>5.0171665534233002E-2</v>
       </c>
       <c r="F172">
         <v>12</v>
       </c>
       <c r="G172">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="H172">
-        <v>0.62528118257478105</v>
+        <v>0.340896561479823</v>
       </c>
       <c r="I172">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J172" t="s">
         <v>41</v>
@@ -7934,7 +8005,7 @@
     </row>
     <row r="173" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="B173" t="s">
         <v>9</v>
@@ -7943,22 +8014,22 @@
         <v>10</v>
       </c>
       <c r="D173">
-        <v>-0.159251159587734</v>
+        <v>-0.16047495227969399</v>
       </c>
       <c r="E173">
-        <v>0.28518099150100101</v>
+        <v>0.152870811915367</v>
       </c>
       <c r="F173">
         <v>12</v>
       </c>
       <c r="G173">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="H173">
-        <v>0.60063823593322496</v>
+        <v>0.341903080736987</v>
       </c>
       <c r="I173">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J173" t="s">
         <v>41</v>
@@ -7966,7 +8037,7 @@
     </row>
     <row r="174" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="B174" t="s">
         <v>9</v>
@@ -7975,10 +8046,10 @@
         <v>10</v>
       </c>
       <c r="D174">
-        <v>-4.54634216259878E-2</v>
+        <v>7.7158883332315298E-2</v>
       </c>
       <c r="E174">
-        <v>0.30800478897245998</v>
+        <v>7.4557702561397696E-2</v>
       </c>
       <c r="F174">
         <v>12</v>
@@ -7987,10 +8058,10 @@
         <v>12</v>
       </c>
       <c r="H174">
-        <v>0.88842116872357002</v>
+        <v>0.34815532851744702</v>
       </c>
       <c r="I174">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J174" t="s">
         <v>41</v>
@@ -7998,7 +8069,7 @@
     </row>
     <row r="175" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="B175" t="s">
         <v>9</v>
@@ -8007,22 +8078,22 @@
         <v>10</v>
       </c>
       <c r="D175">
-        <v>-4.2955816024014402E-2</v>
+        <v>-4.6444422856050504E-3</v>
       </c>
       <c r="E175">
-        <v>0.33168996915464299</v>
+        <v>4.6444422611254602E-3</v>
       </c>
       <c r="F175">
         <v>12</v>
       </c>
       <c r="G175">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="H175">
-        <v>0.90200585649867704</v>
+        <v>0.36321746508783698</v>
       </c>
       <c r="I175">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J175" t="s">
         <v>41</v>
@@ -8030,7 +8101,7 @@
     </row>
     <row r="176" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
-        <v>98</v>
+        <v>111</v>
       </c>
       <c r="B176" t="s">
         <v>9</v>
@@ -8039,22 +8110,22 @@
         <v>10</v>
       </c>
       <c r="D176">
-        <v>-2.7994639488810001E-2</v>
+        <v>0.19930738499376699</v>
       </c>
       <c r="E176">
-        <v>0.14198133807430899</v>
+        <v>0.19930738452635799</v>
       </c>
       <c r="F176">
         <v>12</v>
       </c>
       <c r="G176">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="H176">
-        <v>0.85145810289969304</v>
+        <v>0.36321746643805702</v>
       </c>
       <c r="I176">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J176" t="s">
         <v>41</v>
@@ -8062,7 +8133,7 @@
     </row>
     <row r="177" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
-        <v>35</v>
+        <v>134</v>
       </c>
       <c r="B177" t="s">
         <v>9</v>
@@ -8071,22 +8142,22 @@
         <v>10</v>
       </c>
       <c r="D177">
-        <v>-6.4629698896265894E-2</v>
+        <v>2.1648216758167201E-2</v>
       </c>
       <c r="E177">
-        <v>0.20515187221262199</v>
+        <v>2.17143661021598E-2</v>
       </c>
       <c r="F177">
         <v>12</v>
       </c>
       <c r="G177">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="H177">
-        <v>0.75921166634284498</v>
+        <v>0.36455794549113102</v>
       </c>
       <c r="I177">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J177" t="s">
         <v>41</v>
@@ -8094,7 +8165,7 @@
     </row>
     <row r="178" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="B178" t="s">
         <v>9</v>
@@ -8103,10 +8174,10 @@
         <v>10</v>
       </c>
       <c r="D178">
-        <v>-8.9432236705661694E-2</v>
+        <v>5.75873371518014E-2</v>
       </c>
       <c r="E178">
-        <v>0.22336499638677701</v>
+        <v>5.8019861834660999E-2</v>
       </c>
       <c r="F178">
         <v>12</v>
@@ -8115,10 +8186,10 @@
         <v>12</v>
       </c>
       <c r="H178">
-        <v>0.70540644731532098</v>
+        <v>0.36650501054509499</v>
       </c>
       <c r="I178">
-        <v>0.92161467946604003</v>
+        <v>0.62943251811005396</v>
       </c>
       <c r="J178" t="s">
         <v>41</v>
@@ -8126,7 +8197,7 @@
     </row>
     <row r="179" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
-        <v>102</v>
+        <v>33</v>
       </c>
       <c r="B179" t="s">
         <v>9</v>
@@ -8135,10 +8206,10 @@
         <v>10</v>
       </c>
       <c r="D179">
-        <v>-6.4719611158260797E-3</v>
+        <v>8.5758482931993299E-2</v>
       </c>
       <c r="E179">
-        <v>0.162642126567525</v>
+        <v>8.8557757861333006E-2</v>
       </c>
       <c r="F179">
         <v>12</v>
@@ -8147,10 +8218,10 @@
         <v>12</v>
       </c>
       <c r="H179">
-        <v>0.96979845213923299</v>
+        <v>0.37732568109835701</v>
       </c>
       <c r="I179">
-        <v>0.96979845213923299</v>
+        <v>0.634228272484472</v>
       </c>
       <c r="J179" t="s">
         <v>41</v>
@@ -8158,7 +8229,7 @@
     </row>
     <row r="180" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="B180" t="s">
         <v>9</v>
@@ -8167,30 +8238,30 @@
         <v>10</v>
       </c>
       <c r="D180">
-        <v>-9.1583072825188697E-2</v>
+        <v>4.9850672212000298E-2</v>
       </c>
       <c r="E180">
-        <v>5.7599446600679997E-2</v>
+        <v>5.3064978950686903E-2</v>
       </c>
       <c r="F180">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G180">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H180">
-        <v>0.18653392257123799</v>
+        <v>0.39064180804634002</v>
       </c>
       <c r="I180">
-        <v>0.86038947505113905</v>
+        <v>0.64293130907626805</v>
       </c>
       <c r="J180" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="181" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B181" t="s">
         <v>9</v>
@@ -8199,30 +8270,30 @@
         <v>10</v>
       </c>
       <c r="D181">
-        <v>0.239720906194691</v>
+        <v>8.9255680023123105E-2</v>
       </c>
       <c r="E181">
-        <v>0.15750603776310401</v>
+        <v>0.102364942152493</v>
       </c>
       <c r="F181">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G181">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="H181">
-        <v>0.17816971642037399</v>
+        <v>0.42312833550379603</v>
       </c>
       <c r="I181">
-        <v>0.86038947505113905</v>
+        <v>0.68218650009795601</v>
       </c>
       <c r="J181" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="182" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
-        <v>40</v>
+        <v>66</v>
       </c>
       <c r="B182" t="s">
         <v>9</v>
@@ -8231,30 +8302,30 @@
         <v>10</v>
       </c>
       <c r="D182">
-        <v>0.49393129575448302</v>
+        <v>0.105746489167792</v>
       </c>
       <c r="E182">
-        <v>0.23235975956423799</v>
+        <v>0.123771451044104</v>
       </c>
       <c r="F182">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G182">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H182">
-        <v>0.10260797343581</v>
+        <v>0.43192059316512399</v>
       </c>
       <c r="I182">
-        <v>0.86038947505113905</v>
+        <v>0.68243453720089697</v>
       </c>
       <c r="J182" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="183" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
-        <v>117</v>
+        <v>61</v>
       </c>
       <c r="B183" t="s">
         <v>9</v>
@@ -8263,30 +8334,30 @@
         <v>10</v>
       </c>
       <c r="D183">
-        <v>6.0205999132794702E-2</v>
+        <v>5.6670680195997199E-2</v>
       </c>
       <c r="E183">
-        <v>5.4346204365400101E-2</v>
+        <v>6.7994906940615898E-2</v>
       </c>
       <c r="F183">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G183">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H183">
-        <v>0.296686025879703</v>
+        <v>0.442569463055421</v>
       </c>
       <c r="I183">
-        <v>0.86038947505113905</v>
+        <v>0.68278942008398602</v>
       </c>
       <c r="J183" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="184" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
-        <v>99</v>
+        <v>135</v>
       </c>
       <c r="B184" t="s">
         <v>9</v>
@@ -8295,30 +8366,30 @@
         <v>10</v>
       </c>
       <c r="D184">
-        <v>0.31551632141286801</v>
+        <v>7.1357555081645999E-2</v>
       </c>
       <c r="E184">
-        <v>0.166346056387214</v>
+        <v>8.7002303309637305E-2</v>
       </c>
       <c r="F184">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G184">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H184">
-        <v>0.12523445604545499</v>
+        <v>0.44943101068819302</v>
       </c>
       <c r="I184">
-        <v>0.86038947505113905</v>
+        <v>0.68278942008398602</v>
       </c>
       <c r="J184" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="185" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
-        <v>18</v>
+        <v>136</v>
       </c>
       <c r="B185" t="s">
         <v>9</v>
@@ -8327,30 +8398,30 @@
         <v>10</v>
       </c>
       <c r="D185">
-        <v>8.9189053568095894E-2</v>
+        <v>6.8497710134964307E-2</v>
       </c>
       <c r="E185">
-        <v>6.1645369812336703E-2</v>
+        <v>8.8127258988640406E-2</v>
       </c>
       <c r="F185">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G185">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H185">
-        <v>0.221905112423501</v>
+        <v>0.47215979040946698</v>
       </c>
       <c r="I185">
-        <v>0.86038947505113905</v>
+        <v>0.70378534796882697</v>
       </c>
       <c r="J185" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="186" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
-        <v>92</v>
+        <v>137</v>
       </c>
       <c r="B186" t="s">
         <v>9</v>
@@ -8359,30 +8430,30 @@
         <v>10</v>
       </c>
       <c r="D186">
-        <v>0.37909494407793098</v>
+        <v>1.8196355097754701E-2</v>
       </c>
       <c r="E186">
-        <v>0.28172416440914499</v>
+        <v>2.5179475592163901E-2</v>
       </c>
       <c r="F186">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G186">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="H186">
-        <v>0.25484098175880698</v>
+        <v>0.50226224310452605</v>
       </c>
       <c r="I186">
-        <v>0.86038947505113905</v>
+        <v>0.70685124448959202</v>
       </c>
       <c r="J186" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="187" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
-        <v>35</v>
+        <v>92</v>
       </c>
       <c r="B187" t="s">
         <v>9</v>
@@ -8391,30 +8462,30 @@
         <v>10</v>
       </c>
       <c r="D187">
-        <v>-0.15098563174103699</v>
+        <v>0.201747561866469</v>
       </c>
       <c r="E187">
-        <v>0.11412348789271801</v>
+        <v>0.289930673954791</v>
       </c>
       <c r="F187">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G187">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="H187">
-        <v>0.23664468673602501</v>
+        <v>0.50237525905756497</v>
       </c>
       <c r="I187">
-        <v>0.86038947505113905</v>
+        <v>0.70685124448959202</v>
       </c>
       <c r="J187" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="188" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
-        <v>108</v>
+        <v>58</v>
       </c>
       <c r="B188" t="s">
         <v>9</v>
@@ -8423,30 +8494,30 @@
         <v>10</v>
       </c>
       <c r="D188">
-        <v>0.18062472758293499</v>
+        <v>6.4076935908557203E-2</v>
       </c>
       <c r="E188">
-        <v>0.14226240265996801</v>
+        <v>9.0840778753382007E-2</v>
       </c>
       <c r="F188">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G188">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="H188">
-        <v>0.27665192904955699</v>
+        <v>0.51207179783136403</v>
       </c>
       <c r="I188">
-        <v>0.86038947505113905</v>
+        <v>0.70685124448959202</v>
       </c>
       <c r="J188" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="189" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="B189" t="s">
         <v>9</v>
@@ -8455,30 +8526,30 @@
         <v>10</v>
       </c>
       <c r="D189">
-        <v>-0.21760887771262799</v>
+        <v>-7.4602703262255293E-2</v>
       </c>
       <c r="E189">
-        <v>0.123951745182544</v>
+        <v>0.105905576706892</v>
       </c>
       <c r="F189">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G189">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="H189">
-        <v>0.13559800978543701</v>
+        <v>0.51261446840409797</v>
       </c>
       <c r="I189">
-        <v>0.86038947505113905</v>
+        <v>0.70685124448959202</v>
       </c>
       <c r="J189" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="190" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
-        <v>78</v>
+        <v>32</v>
       </c>
       <c r="B190" t="s">
         <v>9</v>
@@ -8487,30 +8558,30 @@
         <v>10</v>
       </c>
       <c r="D190">
-        <v>-0.17728893797142201</v>
+        <v>-0.106906317391729</v>
       </c>
       <c r="E190">
-        <v>0.20220327636712901</v>
+        <v>0.159922503445633</v>
       </c>
       <c r="F190">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G190">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H190">
-        <v>0.40339910044181798</v>
+        <v>0.51895407823286499</v>
       </c>
       <c r="I190">
-        <v>0.94539913304951095</v>
+        <v>0.70685124448959202</v>
       </c>
       <c r="J190" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="191" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
-        <v>98</v>
+        <v>17</v>
       </c>
       <c r="B191" t="s">
         <v>9</v>
@@ -8519,30 +8590,30 @@
         <v>10</v>
       </c>
       <c r="D191">
-        <v>-0.11008409647811</v>
+        <v>-8.8748401386957901E-2</v>
       </c>
       <c r="E191">
-        <v>0.119042887028775</v>
+        <v>0.13649652579409599</v>
       </c>
       <c r="F191">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G191">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="H191">
-        <v>0.40166477704569797</v>
+        <v>0.54425797842032797</v>
       </c>
       <c r="I191">
-        <v>0.94539913304951095</v>
+        <v>0.72875220839332</v>
       </c>
       <c r="J191" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="192" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
-        <v>118</v>
+        <v>63</v>
       </c>
       <c r="B192" t="s">
         <v>9</v>
@@ -8551,30 +8622,30 @@
         <v>10</v>
       </c>
       <c r="D192">
-        <v>0.14915442688274</v>
+        <v>8.6540805012475602E-2</v>
       </c>
       <c r="E192">
-        <v>0.17801783797372001</v>
+        <v>0.14107097899183599</v>
       </c>
       <c r="F192">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G192">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H192">
-        <v>0.42379961136702199</v>
+        <v>0.566405421921096</v>
       </c>
       <c r="I192">
-        <v>0.94539913304951095</v>
+        <v>0.74576713886277601</v>
       </c>
       <c r="J192" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="193" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="B193" t="s">
         <v>9</v>
@@ -8583,30 +8654,30 @@
         <v>10</v>
       </c>
       <c r="D193">
-        <v>9.0922045190742304E-2</v>
+        <v>2.18197655966949E-2</v>
       </c>
       <c r="E193">
-        <v>0.15110625763150801</v>
+        <v>3.6846479237502401E-2</v>
       </c>
       <c r="F193">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G193">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="H193">
-        <v>0.60096933681379405</v>
+        <v>0.57949194817309901</v>
       </c>
       <c r="I193">
-        <v>0.99321501455163996</v>
+        <v>0.750489572224178</v>
       </c>
       <c r="J193" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="194" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="B194" t="s">
         <v>9</v>
@@ -8615,30 +8686,30 @@
         <v>10</v>
       </c>
       <c r="D194">
-        <v>-0.14560803502362801</v>
+        <v>-0.10769917076427001</v>
       </c>
       <c r="E194">
-        <v>0.33856168688296501</v>
+        <v>0.18684996427022099</v>
       </c>
       <c r="F194">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G194">
         <v>8</v>
       </c>
       <c r="H194">
-        <v>0.684975872104579</v>
+        <v>0.58932294164657995</v>
       </c>
       <c r="I194">
-        <v>0.99321501455163996</v>
+        <v>0.75091149016257797</v>
       </c>
       <c r="J194" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="195" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
-        <v>31</v>
+        <v>89</v>
       </c>
       <c r="B195" t="s">
         <v>9</v>
@@ -8647,30 +8718,30 @@
         <v>10</v>
       </c>
       <c r="D195">
-        <v>-0.16419433866417299</v>
+        <v>-3.11483963789955E-2</v>
       </c>
       <c r="E195">
-        <v>0.21531707023192401</v>
+        <v>6.8939428674976502E-2</v>
       </c>
       <c r="F195">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G195">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H195">
-        <v>0.48445528347283701</v>
+        <v>0.67032130754816099</v>
       </c>
       <c r="I195">
-        <v>0.99321501455163996</v>
+        <v>0.84056163962388497</v>
       </c>
       <c r="J195" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="196" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B196" t="s">
         <v>9</v>
@@ -8679,25 +8750,25 @@
         <v>10</v>
       </c>
       <c r="D196">
-        <v>5.3457364399535703E-2</v>
+        <v>-3.74717641896892E-2</v>
       </c>
       <c r="E196">
-        <v>0.100994686948566</v>
+        <v>9.0294983405063103E-2</v>
       </c>
       <c r="F196">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G196">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="H196">
-        <v>0.62456334040478401</v>
+        <v>0.69535322076138095</v>
       </c>
       <c r="I196">
-        <v>0.99321501455163996</v>
+        <v>0.85302664915152104</v>
       </c>
       <c r="J196" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="197" spans="1:10" x14ac:dyDescent="0.2">
@@ -8711,30 +8782,30 @@
         <v>10</v>
       </c>
       <c r="D197">
-        <v>-2.0092060880896E-2</v>
+        <v>-2.2368429296343199E-2</v>
       </c>
       <c r="E197">
-        <v>3.4389738222720401E-2</v>
+        <v>5.5158350278842701E-2</v>
       </c>
       <c r="F197">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G197">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H197">
-        <v>0.59000813356597104</v>
+        <v>0.70185736955504896</v>
       </c>
       <c r="I197">
-        <v>0.99321501455163996</v>
+        <v>0.85302664915152104</v>
       </c>
       <c r="J197" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="198" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
-        <v>102</v>
+        <v>138</v>
       </c>
       <c r="B198" t="s">
         <v>9</v>
@@ -8743,30 +8814,30 @@
         <v>10</v>
       </c>
       <c r="D198">
-        <v>2.44710313192638E-2</v>
+        <v>4.0917972002572398E-2</v>
       </c>
       <c r="E198">
-        <v>4.4533580972859102E-2</v>
+        <v>0.124054216159714</v>
       </c>
       <c r="F198">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G198">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H198">
-        <v>0.60964172669611405</v>
+        <v>0.75489162260943898</v>
       </c>
       <c r="I198">
-        <v>0.99321501455163996</v>
+        <v>0.87656761595669597</v>
       </c>
       <c r="J198" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="199" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="B199" t="s">
         <v>9</v>
@@ -8775,30 +8846,30 @@
         <v>10</v>
       </c>
       <c r="D199">
-        <v>7.2135673658567503E-2</v>
+        <v>-3.40371336787514E-2</v>
       </c>
       <c r="E199">
-        <v>0.157531619041995</v>
+        <v>0.109814819902865</v>
       </c>
       <c r="F199">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G199">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="H199">
-        <v>0.65787024288597495</v>
+        <v>0.76910105739752599</v>
       </c>
       <c r="I199">
-        <v>0.99321501455163996</v>
+        <v>0.87656761595669597</v>
       </c>
       <c r="J199" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="200" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
-        <v>58</v>
+        <v>35</v>
       </c>
       <c r="B200" t="s">
         <v>9</v>
@@ -8807,30 +8878,30 @@
         <v>10</v>
       </c>
       <c r="D200">
-        <v>2.71962188685935E-2</v>
+        <v>-5.0621432520715701E-2</v>
       </c>
       <c r="E200">
-        <v>0.36024195481072402</v>
+        <v>0.17429211109776299</v>
       </c>
       <c r="F200">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G200">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="H200">
-        <v>0.94276820936170502</v>
+        <v>0.77741345794213301</v>
       </c>
       <c r="I200">
-        <v>0.99998418474858197</v>
+        <v>0.87656761595669597</v>
       </c>
       <c r="J200" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="201" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
-        <v>110</v>
+        <v>44</v>
       </c>
       <c r="B201" t="s">
         <v>9</v>
@@ -8839,30 +8910,30 @@
         <v>10</v>
       </c>
       <c r="D201">
-        <v>-1.6099019597328301E-2</v>
+        <v>3.9015606228173801E-2</v>
       </c>
       <c r="E201">
-        <v>0.17437106237393099</v>
+        <v>0.139538372449656</v>
       </c>
       <c r="F201">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G201">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H201">
-        <v>0.92846132636137502</v>
+        <v>0.79097827340706495</v>
       </c>
       <c r="I201">
-        <v>0.99998418474858197</v>
+        <v>0.87656761595669597</v>
       </c>
       <c r="J201" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="202" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
-        <v>60</v>
+        <v>108</v>
       </c>
       <c r="B202" t="s">
         <v>9</v>
@@ -8871,30 +8942,30 @@
         <v>10</v>
       </c>
       <c r="D202">
-        <v>5.6113704786211999E-2</v>
+        <v>4.5056596198078801E-2</v>
       </c>
       <c r="E202">
-        <v>0.171971813938501</v>
+        <v>0.16397129053473899</v>
       </c>
       <c r="F202">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G202">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H202">
-        <v>0.76003561005793197</v>
+        <v>0.79447504918880896</v>
       </c>
       <c r="I202">
-        <v>0.99998418474858197</v>
+        <v>0.87656761595669597</v>
       </c>
       <c r="J202" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="203" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="B203" t="s">
         <v>9</v>
@@ -8903,30 +8974,30 @@
         <v>10</v>
       </c>
       <c r="D203">
-        <v>5.5647551245440203E-3</v>
+        <v>-8.0826328628377006E-2</v>
       </c>
       <c r="E203">
-        <v>0.11555771067489901</v>
+        <v>0.29970324093089201</v>
       </c>
       <c r="F203">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G203">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="H203">
-        <v>0.96383915533600295</v>
+        <v>0.79817662323029703</v>
       </c>
       <c r="I203">
-        <v>0.99998418474858197</v>
+        <v>0.87656761595669597</v>
       </c>
       <c r="J203" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="204" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
-        <v>25</v>
+        <v>139</v>
       </c>
       <c r="B204" t="s">
         <v>9</v>
@@ -8935,30 +9006,30 @@
         <v>10</v>
       </c>
       <c r="D204">
-        <v>9.4166145353655802E-3</v>
+        <v>2.7295367753106699E-2</v>
       </c>
       <c r="E204">
-        <v>8.1811228631222394E-2</v>
+        <v>0.101584164092242</v>
       </c>
       <c r="F204">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G204">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="H204">
-        <v>0.91391526159089498</v>
+        <v>0.79889706770736901</v>
       </c>
       <c r="I204">
-        <v>0.99998418474858197</v>
+        <v>0.87656761595669597</v>
       </c>
       <c r="J204" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="205" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
-        <v>104</v>
+        <v>140</v>
       </c>
       <c r="B205" t="s">
         <v>9</v>
@@ -8967,30 +9038,30 @@
         <v>10</v>
       </c>
       <c r="D205">
-        <v>7.2068677658347305E-2</v>
+        <v>2.1932010000458701E-2</v>
       </c>
       <c r="E205">
-        <v>0.212899356094643</v>
+        <v>8.6932653749781194E-2</v>
       </c>
       <c r="F205">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G205">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="H205">
-        <v>0.74864917714718004</v>
+        <v>0.810861630031667</v>
       </c>
       <c r="I205">
-        <v>0.99998418474858197</v>
+        <v>0.87750779140413304</v>
       </c>
       <c r="J205" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="206" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
-        <v>28</v>
+        <v>104</v>
       </c>
       <c r="B206" t="s">
         <v>9</v>
@@ -8999,30 +9070,30 @@
         <v>10</v>
       </c>
       <c r="D206">
-        <v>-1.1629532986126101E-2</v>
+        <v>1.6274988764076698E-2</v>
       </c>
       <c r="E206">
-        <v>0.29036118608271699</v>
+        <v>7.0074440647956607E-2</v>
       </c>
       <c r="F206">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G206">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="H206">
-        <v>0.96972718899023902</v>
+        <v>0.82554850307731498</v>
       </c>
       <c r="I206">
-        <v>0.99998418474858197</v>
+        <v>0.87987278231474897</v>
       </c>
       <c r="J206" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="207" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
-        <v>119</v>
+        <v>60</v>
       </c>
       <c r="B207" t="s">
         <v>9</v>
@@ -9030,58 +9101,1050 @@
       <c r="C207" t="s">
         <v>10</v>
       </c>
-      <c r="D207" s="22">
-        <v>-5.2429729796395198E-11</v>
-      </c>
-      <c r="E207" s="22">
-        <v>1.8727969628604699E-6</v>
+      <c r="D207">
+        <v>3.3988154767669101E-2</v>
+      </c>
+      <c r="E207">
+        <v>0.155209800278553</v>
       </c>
       <c r="F207">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G207">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="H207">
-        <v>0.99998418474858197</v>
+        <v>0.83532226169121804</v>
       </c>
       <c r="I207">
-        <v>0.99998418474858197</v>
+        <v>0.87987278231474897</v>
       </c>
       <c r="J207" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="208" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
+        <v>101</v>
+      </c>
+      <c r="B208" t="s">
+        <v>9</v>
+      </c>
+      <c r="C208" t="s">
+        <v>10</v>
+      </c>
+      <c r="D208">
+        <v>-1.1817236929045301E-2</v>
+      </c>
+      <c r="E208">
+        <v>7.1827421374773007E-2</v>
+      </c>
+      <c r="F208">
+        <v>12</v>
+      </c>
+      <c r="G208">
+        <v>12</v>
+      </c>
+      <c r="H208">
+        <v>0.87576403977274897</v>
+      </c>
+      <c r="I208">
+        <v>0.910333672921673</v>
+      </c>
+      <c r="J208" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="209" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A209" t="s">
+        <v>114</v>
+      </c>
+      <c r="B209" t="s">
+        <v>9</v>
+      </c>
+      <c r="C209" t="s">
+        <v>10</v>
+      </c>
+      <c r="D209">
+        <v>1.9161563758151302E-2</v>
+      </c>
+      <c r="E209">
+        <v>0.13604926425350899</v>
+      </c>
+      <c r="F209">
+        <v>12</v>
+      </c>
+      <c r="G209">
+        <v>6</v>
+      </c>
+      <c r="H209">
+        <v>0.89349245355167595</v>
+      </c>
+      <c r="I209">
+        <v>0.91670004974782304</v>
+      </c>
+      <c r="J209" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="210" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A210" t="s">
+        <v>110</v>
+      </c>
+      <c r="B210" t="s">
+        <v>9</v>
+      </c>
+      <c r="C210" t="s">
+        <v>10</v>
+      </c>
+      <c r="D210">
+        <v>1.71110857794495E-4</v>
+      </c>
+      <c r="E210">
+        <v>5.4364013220079402E-2</v>
+      </c>
+      <c r="F210">
+        <v>12</v>
+      </c>
+      <c r="G210">
+        <v>6</v>
+      </c>
+      <c r="H210">
+        <v>0.99761037885803305</v>
+      </c>
+      <c r="I210">
+        <v>0.999844862336983</v>
+      </c>
+      <c r="J210" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="211" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A211" t="s">
+        <v>18</v>
+      </c>
+      <c r="B211" t="s">
+        <v>9</v>
+      </c>
+      <c r="C211" t="s">
+        <v>10</v>
+      </c>
+      <c r="D211" s="22">
+        <v>-3.20963585658992E-5</v>
+      </c>
+      <c r="E211">
+        <v>0.15707329956322</v>
+      </c>
+      <c r="F211">
+        <v>12</v>
+      </c>
+      <c r="G211">
+        <v>12</v>
+      </c>
+      <c r="H211">
+        <v>0.999844862336983</v>
+      </c>
+      <c r="I211">
+        <v>0.999844862336983</v>
+      </c>
+      <c r="J211" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="212" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A212" t="s">
+        <v>11</v>
+      </c>
+      <c r="B212" t="s">
+        <v>9</v>
+      </c>
+      <c r="C212" t="s">
+        <v>10</v>
+      </c>
+      <c r="D212">
+        <v>-4.5999525498556598E-2</v>
+      </c>
+      <c r="E212">
+        <v>2.0879132281052301E-2</v>
+      </c>
+      <c r="F212">
+        <v>11</v>
+      </c>
+      <c r="G212">
+        <v>11</v>
+      </c>
+      <c r="H212">
+        <v>9.4642462177382702E-2</v>
+      </c>
+      <c r="I212">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J212" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="213" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A213" t="s">
+        <v>101</v>
+      </c>
+      <c r="B213" t="s">
+        <v>9</v>
+      </c>
+      <c r="C213" t="s">
+        <v>10</v>
+      </c>
+      <c r="D213">
+        <v>0.121635741253658</v>
+      </c>
+      <c r="E213">
+        <v>5.6758971817264699E-2</v>
+      </c>
+      <c r="F213">
+        <v>11</v>
+      </c>
+      <c r="G213">
+        <v>11</v>
+      </c>
+      <c r="H213">
+        <v>9.7568039062805201E-2</v>
+      </c>
+      <c r="I213">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J213" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="214" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A214" t="s">
+        <v>31</v>
+      </c>
+      <c r="B214" t="s">
+        <v>9</v>
+      </c>
+      <c r="C214" t="s">
+        <v>10</v>
+      </c>
+      <c r="D214">
+        <v>-0.22774699203071999</v>
+      </c>
+      <c r="E214">
+        <v>0.10329115323499501</v>
+      </c>
+      <c r="F214">
+        <v>11</v>
+      </c>
+      <c r="G214">
+        <v>6</v>
+      </c>
+      <c r="H214">
+        <v>9.1476092133328704E-2</v>
+      </c>
+      <c r="I214">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J214" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="215" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A215" t="s">
+        <v>44</v>
+      </c>
+      <c r="B215" t="s">
+        <v>9</v>
+      </c>
+      <c r="C215" t="s">
+        <v>10</v>
+      </c>
+      <c r="D215">
+        <v>-9.89301042098958E-2</v>
+      </c>
+      <c r="E215">
+        <v>5.5831234711556703E-2</v>
+      </c>
+      <c r="F215">
+        <v>11</v>
+      </c>
+      <c r="G215">
+        <v>5</v>
+      </c>
+      <c r="H215">
+        <v>0.15018698052815799</v>
+      </c>
+      <c r="I215">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J215" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="216" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A216" t="s">
+        <v>40</v>
+      </c>
+      <c r="B216" t="s">
+        <v>9</v>
+      </c>
+      <c r="C216" t="s">
+        <v>10</v>
+      </c>
+      <c r="D216">
+        <v>0.44503205256731798</v>
+      </c>
+      <c r="E216">
+        <v>0.256703774698264</v>
+      </c>
+      <c r="F216">
+        <v>11</v>
+      </c>
+      <c r="G216">
+        <v>11</v>
+      </c>
+      <c r="H216">
+        <v>0.161536430984312</v>
+      </c>
+      <c r="I216">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J216" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="217" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A217" t="s">
+        <v>42</v>
+      </c>
+      <c r="B217" t="s">
+        <v>9</v>
+      </c>
+      <c r="C217" t="s">
+        <v>10</v>
+      </c>
+      <c r="D217">
+        <v>-0.20049524538314101</v>
+      </c>
+      <c r="E217">
+        <v>0.144044391514629</v>
+      </c>
+      <c r="F217">
+        <v>11</v>
+      </c>
+      <c r="G217">
+        <v>4</v>
+      </c>
+      <c r="H217">
+        <v>0.229549450055657</v>
+      </c>
+      <c r="I217">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J217" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="218" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A218" t="s">
+        <v>32</v>
+      </c>
+      <c r="B218" t="s">
+        <v>9</v>
+      </c>
+      <c r="C218" t="s">
+        <v>10</v>
+      </c>
+      <c r="D218">
+        <v>6.0205999132797103E-2</v>
+      </c>
+      <c r="E218">
+        <v>5.4346205392122197E-2</v>
+      </c>
+      <c r="F218">
+        <v>11</v>
+      </c>
+      <c r="G218">
+        <v>1</v>
+      </c>
+      <c r="H218">
+        <v>0.296665115826097</v>
+      </c>
+      <c r="I218">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J218" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="219" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A219" t="s">
+        <v>92</v>
+      </c>
+      <c r="B219" t="s">
+        <v>9</v>
+      </c>
+      <c r="C219" t="s">
+        <v>10</v>
+      </c>
+      <c r="D219">
+        <v>0.24224064775849699</v>
+      </c>
+      <c r="E219">
+        <v>0.21411150325460601</v>
+      </c>
+      <c r="F219">
+        <v>11</v>
+      </c>
+      <c r="G219">
+        <v>8</v>
+      </c>
+      <c r="H219">
+        <v>0.33025677998941899</v>
+      </c>
+      <c r="I219">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J219" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="220" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A220" t="s">
+        <v>108</v>
+      </c>
+      <c r="B220" t="s">
+        <v>9</v>
+      </c>
+      <c r="C220" t="s">
+        <v>10</v>
+      </c>
+      <c r="D220">
+        <v>0.123903780269456</v>
+      </c>
+      <c r="E220">
+        <v>0.10939596550283601</v>
+      </c>
+      <c r="F220">
+        <v>11</v>
+      </c>
+      <c r="G220">
+        <v>7</v>
+      </c>
+      <c r="H220">
+        <v>0.32283501218170602</v>
+      </c>
+      <c r="I220">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J220" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="221" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A221" t="s">
+        <v>114</v>
+      </c>
+      <c r="B221" t="s">
+        <v>9</v>
+      </c>
+      <c r="C221" t="s">
+        <v>10</v>
+      </c>
+      <c r="D221">
+        <v>6.0205999132796E-2</v>
+      </c>
+      <c r="E221">
+        <v>5.4346205185996303E-2</v>
+      </c>
+      <c r="F221">
+        <v>11</v>
+      </c>
+      <c r="G221">
+        <v>1</v>
+      </c>
+      <c r="H221">
+        <v>0.29666547960218098</v>
+      </c>
+      <c r="I221">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J221" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="222" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A222" t="s">
+        <v>76</v>
+      </c>
+      <c r="B222" t="s">
+        <v>9</v>
+      </c>
+      <c r="C222" t="s">
+        <v>10</v>
+      </c>
+      <c r="D222">
+        <v>6.8954854875130103E-2</v>
+      </c>
+      <c r="E222">
+        <v>6.4705598050286306E-2</v>
+      </c>
+      <c r="F222">
+        <v>11</v>
+      </c>
+      <c r="G222">
+        <v>2</v>
+      </c>
+      <c r="H222">
+        <v>0.34171600406609798</v>
+      </c>
+      <c r="I222">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J222" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="223" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A223" t="s">
+        <v>111</v>
+      </c>
+      <c r="B223" t="s">
+        <v>9</v>
+      </c>
+      <c r="C223" t="s">
+        <v>10</v>
+      </c>
+      <c r="D223">
+        <v>0.16706785618774</v>
+      </c>
+      <c r="E223">
+        <v>0.153188214685852</v>
+      </c>
+      <c r="F223">
+        <v>11</v>
+      </c>
+      <c r="G223">
+        <v>2</v>
+      </c>
+      <c r="H223">
+        <v>0.32768996727530197</v>
+      </c>
+      <c r="I223">
+        <v>0.79733734282089597</v>
+      </c>
+      <c r="J223" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="224" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A224" t="s">
+        <v>58</v>
+      </c>
+      <c r="B224" t="s">
+        <v>9</v>
+      </c>
+      <c r="C224" t="s">
+        <v>10</v>
+      </c>
+      <c r="D224">
+        <v>-9.6624923896799095E-2</v>
+      </c>
+      <c r="E224">
+        <v>9.6784252766819207E-2</v>
+      </c>
+      <c r="F224">
+        <v>11</v>
+      </c>
+      <c r="G224">
+        <v>11</v>
+      </c>
+      <c r="H224">
+        <v>0.37027498701524197</v>
+      </c>
+      <c r="I224">
+        <v>0.79751535664821405</v>
+      </c>
+      <c r="J224" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="225" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A225" t="s">
+        <v>98</v>
+      </c>
+      <c r="B225" t="s">
+        <v>9</v>
+      </c>
+      <c r="C225" t="s">
+        <v>10</v>
+      </c>
+      <c r="D225">
+        <v>-0.106904445830611</v>
+      </c>
+      <c r="E225">
+        <v>0.115521152035661</v>
+      </c>
+      <c r="F225">
+        <v>11</v>
+      </c>
+      <c r="G225">
+        <v>2</v>
+      </c>
+      <c r="H225">
+        <v>0.401452555316129</v>
+      </c>
+      <c r="I225">
+        <v>0.802905110632258</v>
+      </c>
+      <c r="J225" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="226" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A226" t="s">
+        <v>78</v>
+      </c>
+      <c r="B226" t="s">
+        <v>9</v>
+      </c>
+      <c r="C226" t="s">
+        <v>10</v>
+      </c>
+      <c r="D226">
+        <v>-0.16896207856687301</v>
+      </c>
+      <c r="E226">
+        <v>0.21556940487860901</v>
+      </c>
+      <c r="F226">
+        <v>11</v>
+      </c>
+      <c r="G226">
+        <v>11</v>
+      </c>
+      <c r="H226">
+        <v>0.46665351680429001</v>
+      </c>
+      <c r="I226">
+        <v>0.81246749805360396</v>
+      </c>
+      <c r="J226" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="227" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A227" t="s">
+        <v>104</v>
+      </c>
+      <c r="B227" t="s">
+        <v>9</v>
+      </c>
+      <c r="C227" t="s">
+        <v>10</v>
+      </c>
+      <c r="D227">
+        <v>0.106035680729992</v>
+      </c>
+      <c r="E227">
+        <v>0.17209722910971301</v>
+      </c>
+      <c r="F227">
+        <v>11</v>
+      </c>
+      <c r="G227">
+        <v>10</v>
+      </c>
+      <c r="H227">
+        <v>0.56800590738550805</v>
+      </c>
+      <c r="I227">
+        <v>0.81246749805360396</v>
+      </c>
+      <c r="J227" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="228" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A228" t="s">
+        <v>60</v>
+      </c>
+      <c r="B228" t="s">
+        <v>9</v>
+      </c>
+      <c r="C228" t="s">
+        <v>10</v>
+      </c>
+      <c r="D228">
+        <v>0.120855500158843</v>
+      </c>
+      <c r="E228">
+        <v>0.170764621632539</v>
+      </c>
+      <c r="F228">
+        <v>11</v>
+      </c>
+      <c r="G228">
+        <v>11</v>
+      </c>
+      <c r="H228">
+        <v>0.51687715022283598</v>
+      </c>
+      <c r="I228">
+        <v>0.81246749805360396</v>
+      </c>
+      <c r="J228" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="229" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A229" t="s">
+        <v>35</v>
+      </c>
+      <c r="B229" t="s">
+        <v>9</v>
+      </c>
+      <c r="C229" t="s">
+        <v>10</v>
+      </c>
+      <c r="D229">
+        <v>-0.16782299265296299</v>
+      </c>
+      <c r="E229">
+        <v>0.29261515144271599</v>
+      </c>
+      <c r="F229">
+        <v>11</v>
+      </c>
+      <c r="G229">
+        <v>7</v>
+      </c>
+      <c r="H229">
+        <v>0.58033392718114596</v>
+      </c>
+      <c r="I229">
+        <v>0.81246749805360396</v>
+      </c>
+      <c r="J229" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="230" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A230" t="s">
+        <v>34</v>
+      </c>
+      <c r="B230" t="s">
+        <v>9</v>
+      </c>
+      <c r="C230" t="s">
+        <v>10</v>
+      </c>
+      <c r="D230">
+        <v>6.5724048439564697E-2</v>
+      </c>
+      <c r="E230">
+        <v>9.9599489143358394E-2</v>
+      </c>
+      <c r="F230">
+        <v>11</v>
+      </c>
+      <c r="G230">
+        <v>11</v>
+      </c>
+      <c r="H230">
+        <v>0.54309929971307302</v>
+      </c>
+      <c r="I230">
+        <v>0.81246749805360396</v>
+      </c>
+      <c r="J230" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="231" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A231" t="s">
+        <v>110</v>
+      </c>
+      <c r="B231" t="s">
+        <v>9</v>
+      </c>
+      <c r="C231" t="s">
+        <v>10</v>
+      </c>
+      <c r="D231">
+        <v>-0.106084321206633</v>
+      </c>
+      <c r="E231">
+        <v>0.158489771774529</v>
+      </c>
+      <c r="F231">
+        <v>11</v>
+      </c>
+      <c r="G231">
+        <v>3</v>
+      </c>
+      <c r="H231">
+        <v>0.52007511741670998</v>
+      </c>
+      <c r="I231">
+        <v>0.81246749805360396</v>
+      </c>
+      <c r="J231" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="232" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A232" t="s">
+        <v>18</v>
+      </c>
+      <c r="B232" t="s">
+        <v>9</v>
+      </c>
+      <c r="C232" t="s">
+        <v>10</v>
+      </c>
+      <c r="D232">
+        <v>-1.4901881666131401E-2</v>
+      </c>
+      <c r="E232">
+        <v>3.90187410750421E-2</v>
+      </c>
+      <c r="F232">
+        <v>11</v>
+      </c>
+      <c r="G232">
+        <v>11</v>
+      </c>
+      <c r="H232">
+        <v>0.72065113371572598</v>
+      </c>
+      <c r="I232">
+        <v>0.89083128139840595</v>
+      </c>
+      <c r="J232" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="233" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A233" t="s">
+        <v>17</v>
+      </c>
+      <c r="B233" t="s">
+        <v>9</v>
+      </c>
+      <c r="C233" t="s">
+        <v>10</v>
+      </c>
+      <c r="D233">
+        <v>-0.102349183398409</v>
+      </c>
+      <c r="E233">
+        <v>0.25340168918810702</v>
+      </c>
+      <c r="F233">
+        <v>11</v>
+      </c>
+      <c r="G233">
+        <v>9</v>
+      </c>
+      <c r="H233">
+        <v>0.70282032663594596</v>
+      </c>
+      <c r="I233">
+        <v>0.89083128139840595</v>
+      </c>
+      <c r="J233" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="234" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A234" t="s">
+        <v>25</v>
+      </c>
+      <c r="B234" t="s">
+        <v>9</v>
+      </c>
+      <c r="C234" t="s">
+        <v>10</v>
+      </c>
+      <c r="D234">
+        <v>2.6270429808139002E-2</v>
+      </c>
+      <c r="E234">
+        <v>7.1521135365984104E-2</v>
+      </c>
+      <c r="F234">
+        <v>11</v>
+      </c>
+      <c r="G234">
+        <v>4</v>
+      </c>
+      <c r="H234">
+        <v>0.73175426686297596</v>
+      </c>
+      <c r="I234">
+        <v>0.89083128139840595</v>
+      </c>
+      <c r="J234" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="235" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A235" t="s">
+        <v>141</v>
+      </c>
+      <c r="B235" t="s">
+        <v>9</v>
+      </c>
+      <c r="C235" t="s">
+        <v>10</v>
+      </c>
+      <c r="D235">
+        <v>-1.9590276059821901E-2</v>
+      </c>
+      <c r="E235">
+        <v>0.10863673810925099</v>
+      </c>
+      <c r="F235">
+        <v>11</v>
+      </c>
+      <c r="G235">
+        <v>9</v>
+      </c>
+      <c r="H235">
+        <v>0.86585744379900298</v>
+      </c>
+      <c r="I235">
+        <v>0.93246186255277297</v>
+      </c>
+      <c r="J235" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="236" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A236" t="s">
+        <v>28</v>
+      </c>
+      <c r="B236" t="s">
+        <v>9</v>
+      </c>
+      <c r="C236" t="s">
+        <v>10</v>
+      </c>
+      <c r="D236">
+        <v>-4.4357493493330097E-2</v>
+      </c>
+      <c r="E236">
+        <v>0.24379896245413599</v>
+      </c>
+      <c r="F236">
+        <v>11</v>
+      </c>
+      <c r="G236">
+        <v>5</v>
+      </c>
+      <c r="H236">
+        <v>0.86361643096904595</v>
+      </c>
+      <c r="I236">
+        <v>0.93246186255277297</v>
+      </c>
+      <c r="J236" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="237" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A237" t="s">
+        <v>19</v>
+      </c>
+      <c r="B237" t="s">
+        <v>9</v>
+      </c>
+      <c r="C237" t="s">
+        <v>10</v>
+      </c>
+      <c r="D237">
+        <v>7.5032740393048705E-2</v>
+      </c>
+      <c r="E237">
+        <v>0.17382926744594501</v>
+      </c>
+      <c r="F237">
+        <v>11</v>
+      </c>
+      <c r="G237">
+        <v>3</v>
+      </c>
+      <c r="H237">
+        <v>0.82484424966500403</v>
+      </c>
+      <c r="I237">
+        <v>0.93246186255277297</v>
+      </c>
+      <c r="J237" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="238" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A238" t="s">
         <v>96</v>
       </c>
-      <c r="B208" t="s">
-        <v>9</v>
-      </c>
-      <c r="C208" t="s">
-        <v>10</v>
-      </c>
-      <c r="D208">
-        <v>2.8295174401673999E-2</v>
-      </c>
-      <c r="E208">
-        <v>0.27405802881152103</v>
-      </c>
-      <c r="F208">
+      <c r="B238" t="s">
+        <v>9</v>
+      </c>
+      <c r="C238" t="s">
+        <v>10</v>
+      </c>
+      <c r="D238">
+        <v>-1.82389336773158E-2</v>
+      </c>
+      <c r="E238">
+        <v>0.22905182395198301</v>
+      </c>
+      <c r="F238">
         <v>11</v>
       </c>
-      <c r="G208">
-        <v>9</v>
-      </c>
-      <c r="H208">
-        <v>0.92210482486330703</v>
-      </c>
-      <c r="I208">
-        <v>0.99998418474858197</v>
-      </c>
-      <c r="J208" t="s">
-        <v>45</v>
+      <c r="G238">
+        <v>10</v>
+      </c>
+      <c r="H238">
+        <v>0.93973321399376697</v>
+      </c>
+      <c r="I238">
+        <v>0.93973321399376697</v>
+      </c>
+      <c r="J238" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="239" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A239" t="s">
+        <v>109</v>
+      </c>
+      <c r="B239" t="s">
+        <v>9</v>
+      </c>
+      <c r="C239" t="s">
+        <v>10</v>
+      </c>
+      <c r="D239">
+        <v>-8.7319831566039403E-3</v>
+      </c>
+      <c r="E239">
+        <v>9.3605846122654698E-2</v>
+      </c>
+      <c r="F239">
+        <v>11</v>
+      </c>
+      <c r="G239">
+        <v>2</v>
+      </c>
+      <c r="H239">
+        <v>0.92772110501529603</v>
+      </c>
+      <c r="I239">
+        <v>0.93973321399376697</v>
+      </c>
+      <c r="J239" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>